<commit_message>
Update load function; Update save function; Update condition part; add check template file; add check database; Update template file; Push testcase in progress
</commit_message>
<xml_diff>
--- a/dcomtestcasegeneration/Source/dcom/bin/Debug/DB_Requirement/RequirementDB____DCOM.xlsx
+++ b/dcomtestcasegeneration/Source/dcom/bin/Debug/DB_Requirement/RequirementDB____DCOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BGSV_EDA2_Automation_Tool_LOCALREPO\dcomtestcasegeneration\DCOMTestcaseGenerationR1.1\Source\dcom\bin\Debug\DB_Requirement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\bosch.com\dfsrb\DfsVN\LOC\Hc\RBVH\20_EDA\04_External\00_Common\02_EDA2\db_BGSV_EDA2_Automation_Tool\DCOM\DB_Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E085085-0307-41A6-8E99-F7D94A9C7449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EB0520-5B1F-4924-95DA-481BCA43E9AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="885" windowWidth="24855" windowHeight="15315" tabRatio="903" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26595" yWindow="480" windowWidth="24855" windowHeight="15315" tabRatio="903" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Common_settings" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="98">
   <si>
     <t>NRC</t>
   </si>
@@ -171,33 +171,6 @@
     <t>DID</t>
   </si>
   <si>
-    <t>0103</t>
-  </si>
-  <si>
-    <t>F120</t>
-  </si>
-  <si>
-    <t>F121</t>
-  </si>
-  <si>
-    <t>F187</t>
-  </si>
-  <si>
-    <t>F18A</t>
-  </si>
-  <si>
-    <t>F18C</t>
-  </si>
-  <si>
-    <t>F190</t>
-  </si>
-  <si>
-    <t>F191</t>
-  </si>
-  <si>
-    <t>F194</t>
-  </si>
-  <si>
     <t>Information</t>
   </si>
   <si>
@@ -279,189 +252,6 @@
     <t>DID name</t>
   </si>
   <si>
-    <t>NetworkInformationDataIdentifier</t>
-  </si>
-  <si>
-    <t>FunctionSpecificationDataIdentifier</t>
-  </si>
-  <si>
-    <t>DiagnosticDefinitionDataIdentifier</t>
-  </si>
-  <si>
-    <t>CHANA_ECUSoftwareVersionNumberDataIdentifier</t>
-  </si>
-  <si>
-    <t>CHANA_ECUHardwareVersionNumberDataIdentifier</t>
-  </si>
-  <si>
-    <t>Part Number</t>
-  </si>
-  <si>
-    <t>System Supplier Identifier</t>
-  </si>
-  <si>
-    <t>ECUSerialNumberDataIdentifier</t>
-  </si>
-  <si>
-    <t>VINDataIdentifier</t>
-  </si>
-  <si>
-    <t>FBL Version Information</t>
-  </si>
-  <si>
-    <t>FBL Requirement Specification</t>
-  </si>
-  <si>
-    <t>Fingerprint</t>
-  </si>
-  <si>
-    <t>Software Number</t>
-  </si>
-  <si>
-    <t>Calibration DataIdentifier</t>
-  </si>
-  <si>
-    <t>vehicle type</t>
-  </si>
-  <si>
-    <t>vehicle configuration</t>
-  </si>
-  <si>
-    <t>ECU Hardware version number</t>
-  </si>
-  <si>
-    <t>Supplier Software number</t>
-  </si>
-  <si>
-    <t>FAB switch</t>
-  </si>
-  <si>
-    <t>TSR switch</t>
-  </si>
-  <si>
-    <t>TLA switch</t>
-  </si>
-  <si>
-    <t>Body_height_wheelhouse_edge</t>
-  </si>
-  <si>
-    <t>Calibration Board Distance</t>
-  </si>
-  <si>
-    <t>Invalid Key Counter</t>
-  </si>
-  <si>
-    <t>Current Calibration Status</t>
-  </si>
-  <si>
-    <t>Current static calibration details</t>
-  </si>
-  <si>
-    <t>Current EOL calibration parameters</t>
-  </si>
-  <si>
-    <t>ECU Temperature</t>
-  </si>
-  <si>
-    <t>Can read the Previuos Calibration result</t>
-  </si>
-  <si>
-    <t>Can read the Previuos Previous result</t>
-  </si>
-  <si>
-    <t>ECU Supplier voltage</t>
-  </si>
-  <si>
-    <t>ProgrammingCounter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ProgrammingAttemptCounter </t>
-  </si>
-  <si>
-    <t>ActiveDiagnosticSessionDataIdentifier</t>
-  </si>
-  <si>
-    <t>Lane Function Configuration</t>
-  </si>
-  <si>
-    <t>F122</t>
-  </si>
-  <si>
-    <t>F189</t>
-  </si>
-  <si>
-    <t>F089</t>
-  </si>
-  <si>
-    <t>F170</t>
-  </si>
-  <si>
-    <t>F171</t>
-  </si>
-  <si>
-    <t>F184</t>
-  </si>
-  <si>
-    <t>F188</t>
-  </si>
-  <si>
-    <t>F123</t>
-  </si>
-  <si>
-    <t>F1F0</t>
-  </si>
-  <si>
-    <t>F1F4</t>
-  </si>
-  <si>
-    <t>F1F1</t>
-  </si>
-  <si>
-    <t>F1F2</t>
-  </si>
-  <si>
-    <t>F1F3</t>
-  </si>
-  <si>
-    <t>F1F5</t>
-  </si>
-  <si>
-    <t>3BAF</t>
-  </si>
-  <si>
-    <t>F1F7</t>
-  </si>
-  <si>
-    <t>F1F8</t>
-  </si>
-  <si>
-    <t>F1F9</t>
-  </si>
-  <si>
-    <t>11B7</t>
-  </si>
-  <si>
-    <t>F1FA</t>
-  </si>
-  <si>
-    <t>F1FB</t>
-  </si>
-  <si>
-    <t>11B5</t>
-  </si>
-  <si>
-    <t>0200</t>
-  </si>
-  <si>
-    <t>0201</t>
-  </si>
-  <si>
-    <t>F1FD</t>
-  </si>
-  <si>
-    <t>F1FE</t>
-  </si>
-  <si>
     <t>Data_Path_Information</t>
   </si>
   <si>
@@ -531,12 +321,6 @@
     <t>// Stop DTC Setting</t>
   </si>
   <si>
-    <t>Physical</t>
-  </si>
-  <si>
-    <t>SID Support</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -550,6 +334,12 @@
   </si>
   <si>
     <t>Current_Voltage</t>
+  </si>
+  <si>
+    <t>Voltage</t>
+  </si>
+  <si>
+    <t>Allow Session</t>
   </si>
 </sst>
 </file>
@@ -1075,7 +865,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -1096,12 +886,12 @@
         <v>27</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>140</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
-        <v>164</v>
+        <v>92</v>
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -1115,14 +905,14 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B5" s="22"/>
       <c r="C5" s="22"/>
@@ -1173,21 +963,21 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
-        <v>165</v>
+        <v>93</v>
       </c>
       <c r="B21" s="22"/>
       <c r="C21" s="20"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="19" t="s">
-        <v>166</v>
+        <v>94</v>
       </c>
       <c r="B22" s="22"/>
       <c r="C22" s="20"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
-        <v>167</v>
+        <v>95</v>
       </c>
       <c r="B23" s="22"/>
       <c r="C23" s="20"/>
@@ -1224,69 +1014,69 @@
     </row>
     <row r="30" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
-        <v>144</v>
+        <v>74</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C30" s="20"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
-        <v>145</v>
+        <v>75</v>
       </c>
       <c r="B31" s="22"/>
       <c r="C31" s="20"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B32" s="22"/>
       <c r="C32" s="20"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="19" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B33" s="22"/>
       <c r="C33" s="20"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B34" s="22"/>
     </row>
     <row r="40" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="19" t="s">
-        <v>146</v>
+        <v>76</v>
       </c>
       <c r="B41" s="22"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="19" t="s">
-        <v>147</v>
+        <v>77</v>
       </c>
       <c r="B42" s="22"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="19" t="s">
-        <v>148</v>
+        <v>78</v>
       </c>
       <c r="B43" s="22"/>
     </row>
     <row r="50" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
-        <v>139</v>
+        <v>69</v>
       </c>
       <c r="B50" s="10" t="s">
         <v>31</v>
@@ -1312,7 +1102,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="19" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B54" s="22"/>
     </row>
@@ -1324,19 +1114,19 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="19" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B56" s="22"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="19" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B57" s="22"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B58" s="22"/>
     </row>
@@ -1348,19 +1138,19 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="19" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B60" s="22"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="19" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B61" s="22"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="19" t="s">
-        <v>141</v>
+        <v>71</v>
       </c>
       <c r="B62" s="22"/>
     </row>
@@ -1377,7 +1167,7 @@
   <dimension ref="A1:V111"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P2" sqref="P1:P1048576"/>
+      <selection activeCell="N7" sqref="N7:N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1413,7 +1203,7 @@
       <c r="B1" s="29"/>
       <c r="E1" s="2"/>
       <c r="F1" s="28" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G1" s="29"/>
       <c r="H1" s="29"/>
@@ -1424,27 +1214,27 @@
       </c>
       <c r="L1" s="29"/>
       <c r="N1" s="28" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="O1" s="29"/>
       <c r="P1" s="29"/>
       <c r="Q1" s="29"/>
       <c r="R1" s="29"/>
       <c r="T1" s="28" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="U1" s="29"/>
     </row>
     <row r="2" spans="1:22" s="11" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="10" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>1</v>
@@ -1463,13 +1253,13 @@
         <v>0</v>
       </c>
       <c r="N2" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>163</v>
+        <v>91</v>
       </c>
       <c r="Q2" s="10" t="s">
         <v>31</v>
@@ -1493,7 +1283,7 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="8" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -1504,14 +1294,14 @@
       </c>
       <c r="L3" s="7"/>
       <c r="N3" s="9" t="s">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="O3" s="14"/>
       <c r="P3" s="14"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="T3" s="9" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="U3" s="7"/>
       <c r="V3" s="6" t="s">
@@ -1534,14 +1324,14 @@
       </c>
       <c r="L4" s="7"/>
       <c r="N4" s="9" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="O4" s="14"/>
       <c r="P4" s="14"/>
       <c r="Q4" s="7"/>
       <c r="R4" s="7"/>
       <c r="T4" s="9" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="U4" s="7"/>
       <c r="V4" s="6" t="s">
@@ -1561,7 +1351,9 @@
         <v>16</v>
       </c>
       <c r="L5" s="7"/>
-      <c r="N5" s="9"/>
+      <c r="N5" s="9" t="s">
+        <v>96</v>
+      </c>
       <c r="O5" s="14"/>
       <c r="P5" s="14"/>
       <c r="Q5" s="7"/>
@@ -1582,7 +1374,9 @@
         <v>17</v>
       </c>
       <c r="L6" s="7"/>
-      <c r="N6" s="9"/>
+      <c r="N6" s="9" t="s">
+        <v>96</v>
+      </c>
       <c r="O6" s="14"/>
       <c r="P6" s="14"/>
       <c r="Q6" s="7"/>
@@ -1810,7 +1604,7 @@
       <c r="I17" s="7"/>
       <c r="J17" s="4"/>
       <c r="K17" s="9" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="L17" s="7"/>
       <c r="N17" s="9"/>
@@ -1847,8 +1641,8 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:V111"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P2" sqref="P1:P1048576"/>
+    <sheetView topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5:N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1884,7 +1678,7 @@
       <c r="B1" s="29"/>
       <c r="E1" s="2"/>
       <c r="F1" s="28" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G1" s="29"/>
       <c r="H1" s="29"/>
@@ -1895,27 +1689,27 @@
       </c>
       <c r="L1" s="29"/>
       <c r="N1" s="28" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="O1" s="29"/>
       <c r="P1" s="29"/>
       <c r="Q1" s="29"/>
       <c r="R1" s="29"/>
       <c r="T1" s="28" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="U1" s="29"/>
     </row>
     <row r="2" spans="1:22" s="11" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="10" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>1</v>
@@ -1934,13 +1728,13 @@
         <v>0</v>
       </c>
       <c r="N2" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>163</v>
+        <v>91</v>
       </c>
       <c r="Q2" s="10" t="s">
         <v>31</v>
@@ -1963,11 +1757,11 @@
         <v>15</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>160</v>
+        <v>90</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="8" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -1985,7 +1779,7 @@
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="T3" s="9" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="U3" s="7"/>
       <c r="V3" s="6" t="s">
@@ -2000,7 +1794,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>159</v>
+        <v>89</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="8" t="s">
@@ -2015,14 +1809,14 @@
       </c>
       <c r="L4" s="7"/>
       <c r="N4" s="9" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="O4" s="14"/>
       <c r="P4" s="14"/>
       <c r="Q4" s="7"/>
       <c r="R4" s="7"/>
       <c r="T4" s="9" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="U4" s="7"/>
       <c r="V4" s="6" t="s">
@@ -2043,7 +1837,7 @@
       </c>
       <c r="L5" s="7"/>
       <c r="N5" s="9" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="O5" s="14"/>
       <c r="P5" s="14"/>
@@ -2066,7 +1860,7 @@
       </c>
       <c r="L6" s="7"/>
       <c r="N6" s="9" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="O6" s="14"/>
       <c r="P6" s="14"/>
@@ -2295,7 +2089,7 @@
       <c r="I17" s="7"/>
       <c r="J17" s="4"/>
       <c r="K17" s="9" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="L17" s="7"/>
       <c r="N17" s="9"/>
@@ -2333,7 +2127,7 @@
   <dimension ref="A1:V111"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P2" sqref="P1:P1048576"/>
+      <selection activeCell="N5" sqref="N5:N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2369,7 +2163,7 @@
       <c r="B1" s="29"/>
       <c r="E1" s="2"/>
       <c r="F1" s="28" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G1" s="29"/>
       <c r="H1" s="29"/>
@@ -2380,27 +2174,27 @@
       </c>
       <c r="L1" s="29"/>
       <c r="N1" s="28" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="O1" s="29"/>
       <c r="P1" s="29"/>
       <c r="Q1" s="29"/>
       <c r="R1" s="29"/>
       <c r="T1" s="28" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="U1" s="29"/>
     </row>
     <row r="2" spans="1:22" s="11" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="10" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>1</v>
@@ -2419,13 +2213,13 @@
         <v>0</v>
       </c>
       <c r="N2" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>163</v>
+        <v>91</v>
       </c>
       <c r="Q2" s="10" t="s">
         <v>31</v>
@@ -2448,11 +2242,11 @@
         <v>15</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>160</v>
+        <v>90</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="8" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -2470,7 +2264,7 @@
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="T3" s="9" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="U3" s="7"/>
       <c r="V3" s="6" t="s">
@@ -2485,7 +2279,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>159</v>
+        <v>89</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="8" t="s">
@@ -2500,14 +2294,14 @@
       </c>
       <c r="L4" s="7"/>
       <c r="N4" s="9" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="O4" s="14"/>
       <c r="P4" s="14"/>
       <c r="Q4" s="7"/>
       <c r="R4" s="7"/>
       <c r="T4" s="9" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="U4" s="7"/>
       <c r="V4" s="6" t="s">
@@ -2528,7 +2322,7 @@
       </c>
       <c r="L5" s="7"/>
       <c r="N5" s="9" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="O5" s="14"/>
       <c r="P5" s="14"/>
@@ -2551,7 +2345,7 @@
       </c>
       <c r="L6" s="7"/>
       <c r="N6" s="9" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="O6" s="14"/>
       <c r="P6" s="14"/>
@@ -2780,7 +2574,7 @@
       <c r="I17" s="7"/>
       <c r="J17" s="4"/>
       <c r="K17" s="9" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="L17" s="7"/>
       <c r="N17" s="9"/>
@@ -2818,7 +2612,7 @@
   <dimension ref="A1:V111"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AA13" sqref="AA13"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2854,7 +2648,7 @@
       <c r="B1" s="29"/>
       <c r="E1" s="2"/>
       <c r="F1" s="28" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G1" s="29"/>
       <c r="H1" s="29"/>
@@ -2865,27 +2659,27 @@
       </c>
       <c r="L1" s="29"/>
       <c r="N1" s="28" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="O1" s="29"/>
       <c r="P1" s="29"/>
       <c r="Q1" s="29"/>
       <c r="R1" s="29"/>
       <c r="T1" s="28" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="U1" s="29"/>
     </row>
     <row r="2" spans="1:22" s="11" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="10" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>1</v>
@@ -2904,13 +2698,13 @@
         <v>0</v>
       </c>
       <c r="N2" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>163</v>
+        <v>91</v>
       </c>
       <c r="Q2" s="10" t="s">
         <v>31</v>
@@ -2933,11 +2727,11 @@
         <v>15</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>160</v>
+        <v>90</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="8" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -2955,7 +2749,7 @@
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="T3" s="9" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="U3" s="7"/>
       <c r="V3" s="6" t="s">
@@ -2970,7 +2764,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>159</v>
+        <v>89</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="8" t="s">
@@ -2985,14 +2779,14 @@
       </c>
       <c r="L4" s="7"/>
       <c r="N4" s="9" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="O4" s="14"/>
       <c r="P4" s="14"/>
       <c r="Q4" s="7"/>
       <c r="R4" s="7"/>
       <c r="T4" s="9" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="U4" s="7"/>
       <c r="V4" s="6" t="s">
@@ -3013,7 +2807,7 @@
       </c>
       <c r="L5" s="7"/>
       <c r="N5" s="9" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="O5" s="14"/>
       <c r="P5" s="14"/>
@@ -3036,7 +2830,7 @@
       </c>
       <c r="L6" s="7"/>
       <c r="N6" s="9" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="O6" s="14"/>
       <c r="P6" s="14"/>
@@ -3265,7 +3059,7 @@
       <c r="I17" s="7"/>
       <c r="J17" s="4"/>
       <c r="K17" s="9" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="L17" s="7"/>
       <c r="N17" s="9"/>
@@ -3303,7 +3097,7 @@
   <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P2" sqref="P1:P1048576"/>
+      <selection activeCell="N5" sqref="N5:N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3339,7 +3133,7 @@
       <c r="B1" s="29"/>
       <c r="E1" s="2"/>
       <c r="F1" s="28" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="G1" s="29"/>
       <c r="H1" s="29"/>
@@ -3350,27 +3144,27 @@
       </c>
       <c r="L1" s="29"/>
       <c r="N1" s="28" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="O1" s="29"/>
       <c r="P1" s="29"/>
       <c r="Q1" s="29"/>
       <c r="R1" s="29"/>
       <c r="T1" s="28" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="U1" s="29"/>
     </row>
     <row r="2" spans="1:22" s="11" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="10" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>1</v>
@@ -3389,13 +3183,13 @@
         <v>0</v>
       </c>
       <c r="N2" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>163</v>
+        <v>91</v>
       </c>
       <c r="Q2" s="10" t="s">
         <v>31</v>
@@ -3419,7 +3213,7 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="8" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -3437,7 +3231,7 @@
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="T3" s="9" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="U3" s="7"/>
       <c r="V3" s="6" t="s">
@@ -3464,14 +3258,14 @@
       </c>
       <c r="L4" s="7"/>
       <c r="N4" s="9" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="O4" s="14"/>
       <c r="P4" s="14"/>
       <c r="Q4" s="7"/>
       <c r="R4" s="7"/>
       <c r="T4" s="9" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="U4" s="7"/>
       <c r="V4" s="6" t="s">
@@ -3487,7 +3281,7 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="8" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -3498,7 +3292,7 @@
       </c>
       <c r="L5" s="7"/>
       <c r="N5" s="9" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="O5" s="14"/>
       <c r="P5" s="14"/>
@@ -3512,7 +3306,7 @@
       <c r="B6" s="9"/>
       <c r="E6" s="2"/>
       <c r="F6" s="8" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
@@ -3523,7 +3317,7 @@
       </c>
       <c r="L6" s="7"/>
       <c r="N6" s="9" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="O6" s="14"/>
       <c r="P6" s="14"/>
@@ -3537,7 +3331,7 @@
       <c r="B7" s="9"/>
       <c r="E7" s="2"/>
       <c r="F7" s="8" t="s">
-        <v>149</v>
+        <v>79</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -3754,7 +3548,7 @@
       <c r="I17" s="7"/>
       <c r="J17" s="4"/>
       <c r="K17" s="9" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="L17" s="7"/>
       <c r="N17" s="9"/>
@@ -3785,7 +3579,7 @@
   <dimension ref="A1:V111"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P2" sqref="P1:P1048576"/>
+      <selection activeCell="N5" sqref="N5:N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3821,7 +3615,7 @@
       <c r="B1" s="29"/>
       <c r="E1" s="2"/>
       <c r="F1" s="28" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G1" s="29"/>
       <c r="H1" s="29"/>
@@ -3832,27 +3626,27 @@
       </c>
       <c r="L1" s="29"/>
       <c r="N1" s="28" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="O1" s="29"/>
       <c r="P1" s="29"/>
       <c r="Q1" s="29"/>
       <c r="R1" s="29"/>
       <c r="T1" s="28" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="U1" s="29"/>
     </row>
     <row r="2" spans="1:22" s="11" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="10" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>1</v>
@@ -3871,13 +3665,13 @@
         <v>0</v>
       </c>
       <c r="N2" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>163</v>
+        <v>91</v>
       </c>
       <c r="Q2" s="10" t="s">
         <v>31</v>
@@ -3899,7 +3693,7 @@
       <c r="B3" s="7"/>
       <c r="E3" s="2"/>
       <c r="F3" s="8" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -3917,7 +3711,7 @@
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="T3" s="9" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="U3" s="7"/>
       <c r="V3" s="6" t="s">
@@ -3942,14 +3736,14 @@
       </c>
       <c r="L4" s="7"/>
       <c r="N4" s="9" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="O4" s="14"/>
       <c r="P4" s="14"/>
       <c r="Q4" s="7"/>
       <c r="R4" s="7"/>
       <c r="T4" s="9" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="U4" s="7"/>
       <c r="V4" s="6" t="s">
@@ -3972,7 +3766,7 @@
       </c>
       <c r="L5" s="7"/>
       <c r="N5" s="9" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="O5" s="14"/>
       <c r="P5" s="14"/>
@@ -3995,7 +3789,7 @@
       </c>
       <c r="L6" s="7"/>
       <c r="N6" s="9" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="O6" s="14"/>
       <c r="P6" s="14"/>
@@ -4224,7 +4018,7 @@
       <c r="I17" s="7"/>
       <c r="J17" s="4"/>
       <c r="K17" s="9" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="L17" s="7"/>
       <c r="N17" s="9"/>
@@ -4262,7 +4056,7 @@
   <dimension ref="A1:V111"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P2" sqref="P1:P1048576"/>
+      <selection activeCell="N5" sqref="N5:N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4298,7 +4092,7 @@
       <c r="B1" s="29"/>
       <c r="E1" s="2"/>
       <c r="F1" s="28" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G1" s="29"/>
       <c r="H1" s="29"/>
@@ -4309,27 +4103,27 @@
       </c>
       <c r="L1" s="29"/>
       <c r="N1" s="28" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="O1" s="29"/>
       <c r="P1" s="29"/>
       <c r="Q1" s="29"/>
       <c r="R1" s="29"/>
       <c r="T1" s="28" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="U1" s="29"/>
     </row>
     <row r="2" spans="1:22" s="11" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="10" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>1</v>
@@ -4348,13 +4142,13 @@
         <v>0</v>
       </c>
       <c r="N2" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>163</v>
+        <v>91</v>
       </c>
       <c r="Q2" s="10" t="s">
         <v>31</v>
@@ -4378,7 +4172,7 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="8" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -4389,14 +4183,14 @@
       </c>
       <c r="L3" s="7"/>
       <c r="N3" s="9" t="s">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="O3" s="14"/>
       <c r="P3" s="14"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="T3" s="9" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="U3" s="7"/>
       <c r="V3" s="6" t="s">
@@ -4419,14 +4213,14 @@
       </c>
       <c r="L4" s="7"/>
       <c r="N4" s="9" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="O4" s="14"/>
       <c r="P4" s="14"/>
       <c r="Q4" s="7"/>
       <c r="R4" s="7"/>
       <c r="T4" s="9" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="U4" s="7"/>
       <c r="V4" s="6" t="s">
@@ -4446,7 +4240,9 @@
         <v>16</v>
       </c>
       <c r="L5" s="7"/>
-      <c r="N5" s="9"/>
+      <c r="N5" s="9" t="s">
+        <v>96</v>
+      </c>
       <c r="O5" s="14"/>
       <c r="P5" s="14"/>
       <c r="Q5" s="7"/>
@@ -4467,7 +4263,9 @@
         <v>17</v>
       </c>
       <c r="L6" s="7"/>
-      <c r="N6" s="9"/>
+      <c r="N6" s="9" t="s">
+        <v>96</v>
+      </c>
       <c r="O6" s="14"/>
       <c r="P6" s="14"/>
       <c r="Q6" s="7"/>
@@ -4695,7 +4493,7 @@
       <c r="I17" s="7"/>
       <c r="J17" s="4"/>
       <c r="K17" s="9" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="L17" s="7"/>
       <c r="N17" s="9"/>
@@ -4733,7 +4531,7 @@
   <dimension ref="A1:V111"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P2" sqref="P1:P1048576"/>
+      <selection activeCell="N5" sqref="N5:N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4769,7 +4567,7 @@
       <c r="D1" s="31"/>
       <c r="E1" s="2"/>
       <c r="F1" s="28" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G1" s="29"/>
       <c r="H1" s="29"/>
@@ -4780,20 +4578,20 @@
       </c>
       <c r="L1" s="29"/>
       <c r="N1" s="28" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="O1" s="29"/>
       <c r="P1" s="29"/>
       <c r="Q1" s="29"/>
       <c r="R1" s="29"/>
       <c r="T1" s="28" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="U1" s="29"/>
     </row>
     <row r="2" spans="1:22" s="11" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4802,7 +4600,7 @@
       <c r="D2" s="10"/>
       <c r="E2" s="12"/>
       <c r="F2" s="10" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>1</v>
@@ -4821,13 +4619,13 @@
         <v>0</v>
       </c>
       <c r="N2" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>163</v>
+        <v>91</v>
       </c>
       <c r="Q2" s="10" t="s">
         <v>31</v>
@@ -4851,7 +4649,7 @@
       <c r="D3" s="14"/>
       <c r="E3" s="2"/>
       <c r="F3" s="8" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -4862,14 +4660,14 @@
       </c>
       <c r="L3" s="7"/>
       <c r="N3" s="9" t="s">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="O3" s="14"/>
       <c r="P3" s="14"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="T3" s="9" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="U3" s="7"/>
       <c r="V3" s="6" t="s">
@@ -4896,14 +4694,14 @@
       </c>
       <c r="L4" s="7"/>
       <c r="N4" s="9" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="O4" s="14"/>
       <c r="P4" s="14"/>
       <c r="Q4" s="7"/>
       <c r="R4" s="7"/>
       <c r="T4" s="9" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="U4" s="7"/>
       <c r="V4" s="6" t="s">
@@ -4927,7 +4725,9 @@
         <v>16</v>
       </c>
       <c r="L5" s="7"/>
-      <c r="N5" s="9"/>
+      <c r="N5" s="9" t="s">
+        <v>96</v>
+      </c>
       <c r="O5" s="14"/>
       <c r="P5" s="14"/>
       <c r="Q5" s="7"/>
@@ -4952,7 +4752,9 @@
         <v>17</v>
       </c>
       <c r="L6" s="7"/>
-      <c r="N6" s="9"/>
+      <c r="N6" s="9" t="s">
+        <v>96</v>
+      </c>
       <c r="O6" s="14"/>
       <c r="P6" s="14"/>
       <c r="Q6" s="7"/>
@@ -5203,7 +5005,7 @@
       <c r="I17" s="7"/>
       <c r="J17" s="4"/>
       <c r="K17" s="9" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="L17" s="7"/>
       <c r="N17" s="9"/>
@@ -5240,8 +5042,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:AD37"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q1:Q1048576"/>
+    <sheetView topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC3" sqref="AC3:AC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5279,7 +5081,7 @@
       <c r="D1" s="31"/>
       <c r="E1" s="2"/>
       <c r="F1" s="28" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G1" s="29"/>
       <c r="H1" s="29"/>
@@ -5291,37 +5093,37 @@
       </c>
       <c r="M1" s="29"/>
       <c r="O1" s="28" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="P1" s="29"/>
       <c r="Q1" s="29"/>
       <c r="R1" s="29"/>
       <c r="S1" s="29"/>
       <c r="U1" s="28" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="V1" s="29"/>
       <c r="AC1" s="28" t="s">
-        <v>162</v>
+        <v>97</v>
       </c>
       <c r="AD1" s="29"/>
     </row>
     <row r="2" spans="1:30" s="11" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>40</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>28</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="10" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>38</v>
@@ -5343,13 +5145,13 @@
         <v>0</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="Q2" s="10" t="s">
-        <v>163</v>
+        <v>91</v>
       </c>
       <c r="R2" s="10" t="s">
         <v>31</v>
@@ -5371,12 +5173,8 @@
       </c>
     </row>
     <row r="3" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>42</v>
-      </c>
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="15"/>
       <c r="D3" s="18"/>
       <c r="E3" s="2"/>
@@ -5391,31 +5189,27 @@
       </c>
       <c r="M3" s="7"/>
       <c r="O3" s="9" t="s">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="P3" s="14"/>
       <c r="Q3" s="14"/>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
       <c r="U3" s="9" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="V3" s="7"/>
       <c r="W3" s="6" t="s">
         <v>37</v>
       </c>
       <c r="AC3" s="9" t="s">
-        <v>161</v>
+        <v>1</v>
       </c>
       <c r="AD3" s="7"/>
     </row>
     <row r="4" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>43</v>
-      </c>
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="15"/>
       <c r="D4" s="18"/>
       <c r="E4" s="2"/>
@@ -5430,31 +5224,27 @@
       </c>
       <c r="M4" s="7"/>
       <c r="O4" s="9" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
       <c r="R4" s="7"/>
       <c r="S4" s="7"/>
       <c r="U4" s="9" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="V4" s="7"/>
       <c r="W4" s="6" t="s">
         <v>36</v>
       </c>
       <c r="AC4" s="9" t="s">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="AD4" s="7"/>
     </row>
     <row r="5" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>112</v>
-      </c>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="15"/>
       <c r="D5" s="18"/>
       <c r="E5" s="2"/>
@@ -5468,23 +5258,23 @@
         <v>16</v>
       </c>
       <c r="M5" s="7"/>
-      <c r="O5" s="9"/>
+      <c r="O5" s="9" t="s">
+        <v>96</v>
+      </c>
       <c r="P5" s="14"/>
       <c r="Q5" s="14"/>
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
       <c r="U5" s="9"/>
       <c r="V5" s="7"/>
-      <c r="AC5" s="9"/>
+      <c r="AC5" s="9" t="s">
+        <v>3</v>
+      </c>
       <c r="AD5" s="7"/>
     </row>
     <row r="6" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>113</v>
-      </c>
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="15"/>
       <c r="D6" s="18"/>
       <c r="E6" s="2"/>
@@ -5498,7 +5288,9 @@
         <v>17</v>
       </c>
       <c r="M6" s="7"/>
-      <c r="O6" s="9"/>
+      <c r="O6" s="9" t="s">
+        <v>96</v>
+      </c>
       <c r="P6" s="14"/>
       <c r="Q6" s="14"/>
       <c r="R6" s="7"/>
@@ -5507,12 +5299,8 @@
       <c r="V6" s="7"/>
     </row>
     <row r="7" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>114</v>
-      </c>
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="18"/>
       <c r="E7" s="2"/>
@@ -5535,12 +5323,8 @@
       <c r="V7" s="7"/>
     </row>
     <row r="8" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>44</v>
-      </c>
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="18"/>
       <c r="E8" s="2"/>
@@ -5563,12 +5347,8 @@
       <c r="V8" s="7"/>
     </row>
     <row r="9" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="18"/>
       <c r="E9" s="3"/>
@@ -5591,12 +5371,8 @@
       <c r="V9" s="7"/>
     </row>
     <row r="10" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>46</v>
-      </c>
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="18"/>
       <c r="E10" s="2"/>
@@ -5619,12 +5395,8 @@
       <c r="V10" s="7"/>
     </row>
     <row r="11" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>47</v>
-      </c>
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="18"/>
       <c r="E11" s="2"/>
@@ -5647,12 +5419,8 @@
       <c r="V11" s="7"/>
     </row>
     <row r="12" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>115</v>
-      </c>
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="15"/>
       <c r="D12" s="18"/>
       <c r="E12" s="2"/>
@@ -5675,12 +5443,8 @@
       <c r="V12" s="7"/>
     </row>
     <row r="13" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>116</v>
-      </c>
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="18"/>
       <c r="E13" s="2"/>
@@ -5703,12 +5467,8 @@
       <c r="V13" s="7"/>
     </row>
     <row r="14" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>117</v>
-      </c>
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
       <c r="C14" s="15"/>
       <c r="D14" s="18"/>
       <c r="E14" s="2"/>
@@ -5731,12 +5491,8 @@
       <c r="V14" s="7"/>
     </row>
     <row r="15" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>118</v>
-      </c>
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="18"/>
       <c r="E15" s="2"/>
@@ -5759,12 +5515,8 @@
       <c r="V15" s="7"/>
     </row>
     <row r="16" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>119</v>
-      </c>
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="18"/>
       <c r="E16" s="2"/>
@@ -5787,12 +5539,8 @@
       <c r="V16" s="7"/>
     </row>
     <row r="17" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>120</v>
-      </c>
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
       <c r="C17" s="15"/>
       <c r="D17" s="18"/>
       <c r="E17" s="4"/>
@@ -5803,7 +5551,7 @@
       <c r="J17" s="7"/>
       <c r="K17" s="4"/>
       <c r="L17" s="9" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="M17" s="7"/>
       <c r="O17" s="9"/>
@@ -5815,12 +5563,8 @@
       <c r="V17" s="7"/>
     </row>
     <row r="18" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>121</v>
-      </c>
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
       <c r="C18" s="16"/>
       <c r="D18" s="18"/>
       <c r="F18" s="7"/>
@@ -5830,12 +5574,8 @@
       <c r="J18" s="7"/>
     </row>
     <row r="19" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>48</v>
-      </c>
+      <c r="A19" s="16"/>
+      <c r="B19" s="16"/>
       <c r="C19" s="16"/>
       <c r="D19" s="18"/>
       <c r="F19" s="7"/>
@@ -5845,12 +5585,8 @@
       <c r="J19" s="7"/>
     </row>
     <row r="20" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>49</v>
-      </c>
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="16"/>
       <c r="D20" s="18"/>
       <c r="F20" s="7"/>
@@ -5860,12 +5596,8 @@
       <c r="J20" s="7"/>
     </row>
     <row r="21" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>122</v>
-      </c>
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
       <c r="C21" s="16"/>
       <c r="D21" s="18"/>
       <c r="F21" s="7"/>
@@ -5875,12 +5607,8 @@
       <c r="J21" s="7"/>
     </row>
     <row r="22" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>123</v>
-      </c>
+      <c r="A22" s="16"/>
+      <c r="B22" s="16"/>
       <c r="C22" s="16"/>
       <c r="D22" s="18"/>
       <c r="F22" s="7"/>
@@ -5890,12 +5618,8 @@
       <c r="J22" s="7"/>
     </row>
     <row r="23" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>124</v>
-      </c>
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
       <c r="C23" s="16"/>
       <c r="D23" s="18"/>
       <c r="F23" s="7"/>
@@ -5905,12 +5629,8 @@
       <c r="J23" s="7"/>
     </row>
     <row r="24" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>125</v>
-      </c>
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
       <c r="C24" s="16"/>
       <c r="D24" s="18"/>
       <c r="F24" s="7"/>
@@ -5920,12 +5640,8 @@
       <c r="J24" s="7"/>
     </row>
     <row r="25" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>126</v>
-      </c>
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
       <c r="C25" s="16"/>
       <c r="D25" s="18"/>
       <c r="F25" s="7"/>
@@ -5935,12 +5651,8 @@
       <c r="J25" s="7"/>
     </row>
     <row r="26" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>41</v>
-      </c>
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
       <c r="C26" s="16"/>
       <c r="D26" s="18"/>
       <c r="F26" s="7"/>
@@ -5950,12 +5662,8 @@
       <c r="J26" s="7"/>
     </row>
     <row r="27" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>127</v>
-      </c>
+      <c r="A27" s="16"/>
+      <c r="B27" s="16"/>
       <c r="C27" s="16"/>
       <c r="D27" s="18"/>
       <c r="F27" s="7"/>
@@ -5965,12 +5673,8 @@
       <c r="J27" s="7"/>
     </row>
     <row r="28" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>128</v>
-      </c>
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
       <c r="C28" s="16"/>
       <c r="D28" s="18"/>
       <c r="F28" s="7"/>
@@ -5980,12 +5684,8 @@
       <c r="J28" s="7"/>
     </row>
     <row r="29" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>129</v>
-      </c>
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="16"/>
       <c r="D29" s="18"/>
       <c r="F29" s="7"/>
@@ -5995,12 +5695,8 @@
       <c r="J29" s="7"/>
     </row>
     <row r="30" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>130</v>
-      </c>
+      <c r="A30" s="16"/>
+      <c r="B30" s="16"/>
       <c r="C30" s="16"/>
       <c r="D30" s="18"/>
       <c r="F30" s="7"/>
@@ -6010,12 +5706,8 @@
       <c r="J30" s="7"/>
     </row>
     <row r="31" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>131</v>
-      </c>
+      <c r="A31" s="16"/>
+      <c r="B31" s="16"/>
       <c r="C31" s="16"/>
       <c r="D31" s="18"/>
       <c r="F31" s="7"/>
@@ -6025,12 +5717,8 @@
       <c r="J31" s="7"/>
     </row>
     <row r="32" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>132</v>
-      </c>
+      <c r="A32" s="16"/>
+      <c r="B32" s="16"/>
       <c r="C32" s="16"/>
       <c r="D32" s="18"/>
       <c r="F32" s="7"/>
@@ -6040,12 +5728,8 @@
       <c r="J32" s="7"/>
     </row>
     <row r="33" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>133</v>
-      </c>
+      <c r="A33" s="16"/>
+      <c r="B33" s="16"/>
       <c r="C33" s="16"/>
       <c r="D33" s="18"/>
       <c r="F33" s="7"/>
@@ -6055,12 +5739,8 @@
       <c r="J33" s="7"/>
     </row>
     <row r="34" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="B34" s="16" t="s">
-        <v>134</v>
-      </c>
+      <c r="A34" s="16"/>
+      <c r="B34" s="16"/>
       <c r="C34" s="16"/>
       <c r="D34" s="18"/>
       <c r="F34" s="7"/>
@@ -6070,12 +5750,8 @@
       <c r="J34" s="7"/>
     </row>
     <row r="35" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="B35" s="16" t="s">
-        <v>135</v>
-      </c>
+      <c r="A35" s="16"/>
+      <c r="B35" s="16"/>
       <c r="C35" s="16"/>
       <c r="D35" s="18"/>
       <c r="F35" s="7"/>
@@ -6085,12 +5761,8 @@
       <c r="J35" s="7"/>
     </row>
     <row r="36" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>136</v>
-      </c>
+      <c r="A36" s="16"/>
+      <c r="B36" s="16"/>
       <c r="C36" s="16"/>
       <c r="D36" s="18"/>
       <c r="F36" s="7"/>
@@ -6100,12 +5772,8 @@
       <c r="J36" s="7"/>
     </row>
     <row r="37" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="B37" s="16" t="s">
-        <v>137</v>
-      </c>
+      <c r="A37" s="16"/>
+      <c r="B37" s="16"/>
       <c r="C37" s="16"/>
       <c r="D37" s="18"/>
       <c r="F37" s="7"/>
@@ -6134,8 +5802,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:AD111"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q1:Q1048576"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AC3" sqref="AC3:AC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6173,7 +5841,7 @@
       <c r="D1" s="31"/>
       <c r="E1" s="2"/>
       <c r="F1" s="28" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G1" s="29"/>
       <c r="H1" s="29"/>
@@ -6185,37 +5853,37 @@
       </c>
       <c r="M1" s="29"/>
       <c r="O1" s="28" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="P1" s="29"/>
       <c r="Q1" s="29"/>
       <c r="R1" s="29"/>
       <c r="S1" s="29"/>
       <c r="U1" s="28" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="V1" s="29"/>
       <c r="AC1" s="28" t="s">
-        <v>162</v>
+        <v>97</v>
       </c>
       <c r="AD1" s="29"/>
     </row>
     <row r="2" spans="1:30" s="11" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>40</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>28</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="10" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>38</v>
@@ -6237,13 +5905,13 @@
         <v>0</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="Q2" s="10" t="s">
-        <v>163</v>
+        <v>91</v>
       </c>
       <c r="R2" s="10" t="s">
         <v>31</v>
@@ -6281,21 +5949,21 @@
       </c>
       <c r="M3" s="7"/>
       <c r="O3" s="9" t="s">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="P3" s="14"/>
       <c r="Q3" s="14"/>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
       <c r="U3" s="9" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="V3" s="7"/>
       <c r="W3" s="6" t="s">
         <v>37</v>
       </c>
       <c r="AC3" s="9" t="s">
-        <v>161</v>
+        <v>1</v>
       </c>
       <c r="AD3" s="7"/>
     </row>
@@ -6316,21 +5984,21 @@
       </c>
       <c r="M4" s="7"/>
       <c r="O4" s="9" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
       <c r="R4" s="7"/>
       <c r="S4" s="7"/>
       <c r="U4" s="9" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="V4" s="7"/>
       <c r="W4" s="6" t="s">
         <v>36</v>
       </c>
       <c r="AC4" s="9" t="s">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="AD4" s="7"/>
     </row>
@@ -6350,14 +6018,18 @@
         <v>16</v>
       </c>
       <c r="M5" s="7"/>
-      <c r="O5" s="9"/>
+      <c r="O5" s="9" t="s">
+        <v>96</v>
+      </c>
       <c r="P5" s="14"/>
       <c r="Q5" s="14"/>
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
       <c r="U5" s="9"/>
       <c r="V5" s="7"/>
-      <c r="AC5" s="9"/>
+      <c r="AC5" s="9" t="s">
+        <v>3</v>
+      </c>
       <c r="AD5" s="7"/>
     </row>
     <row r="6" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6376,7 +6048,9 @@
         <v>17</v>
       </c>
       <c r="M6" s="7"/>
-      <c r="O6" s="9"/>
+      <c r="O6" s="9" t="s">
+        <v>96</v>
+      </c>
       <c r="P6" s="14"/>
       <c r="Q6" s="14"/>
       <c r="R6" s="7"/>
@@ -6637,7 +6311,7 @@
       <c r="J17" s="7"/>
       <c r="K17" s="4"/>
       <c r="L17" s="9" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="M17" s="7"/>
       <c r="O17" s="9"/>
@@ -6896,7 +6570,7 @@
   <dimension ref="A1:W111"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q1:Q1048576"/>
+      <selection activeCell="S44" sqref="S44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6933,7 +6607,7 @@
       <c r="B1" s="29"/>
       <c r="E1" s="2"/>
       <c r="F1" s="28" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G1" s="29"/>
       <c r="H1" s="29"/>
@@ -6945,27 +6619,27 @@
       <c r="L1" s="31"/>
       <c r="M1" s="31"/>
       <c r="O1" s="28" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="P1" s="29"/>
       <c r="Q1" s="29"/>
       <c r="R1" s="29"/>
       <c r="S1" s="29"/>
       <c r="U1" s="28" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="V1" s="29"/>
     </row>
     <row r="2" spans="1:23" s="11" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="10" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>1</v>
@@ -6981,19 +6655,19 @@
         <v>8</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>142</v>
+        <v>72</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>143</v>
+        <v>73</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="Q2" s="10" t="s">
-        <v>163</v>
+        <v>91</v>
       </c>
       <c r="R2" s="10" t="s">
         <v>31</v>
@@ -7017,7 +6691,7 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="8" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -7036,7 +6710,7 @@
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
       <c r="U3" s="9" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="V3" s="7"/>
       <c r="W3" s="6" t="s">
@@ -7064,14 +6738,14 @@
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
       <c r="O4" s="9" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
       <c r="R4" s="7"/>
       <c r="S4" s="7"/>
       <c r="U4" s="9" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="V4" s="7"/>
       <c r="W4" s="6" t="s">
@@ -7093,7 +6767,7 @@
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
       <c r="O5" s="9" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="P5" s="14"/>
       <c r="Q5" s="14"/>
@@ -7117,7 +6791,7 @@
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
       <c r="O6" s="9" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="P6" s="14"/>
       <c r="Q6" s="14"/>
@@ -7356,7 +7030,7 @@
       <c r="I17" s="7"/>
       <c r="J17" s="4"/>
       <c r="K17" s="9" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
@@ -7395,7 +7069,7 @@
   <dimension ref="A1:V111"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P2" sqref="P1:P1048576"/>
+      <selection activeCell="N5" sqref="N5:N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7433,7 +7107,7 @@
       <c r="D1" s="31"/>
       <c r="E1" s="25"/>
       <c r="F1" s="28" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G1" s="29"/>
       <c r="H1" s="29"/>
@@ -7444,33 +7118,33 @@
       </c>
       <c r="L1" s="29"/>
       <c r="N1" s="28" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="O1" s="29"/>
       <c r="P1" s="29"/>
       <c r="Q1" s="29"/>
       <c r="R1" s="29"/>
       <c r="T1" s="28" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="U1" s="29"/>
     </row>
     <row r="2" spans="1:22" s="11" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>155</v>
+        <v>85</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>31</v>
       </c>
       <c r="E2" s="26"/>
       <c r="F2" s="10" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>1</v>
@@ -7489,13 +7163,13 @@
         <v>0</v>
       </c>
       <c r="N2" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>163</v>
+        <v>91</v>
       </c>
       <c r="Q2" s="10" t="s">
         <v>31</v>
@@ -7520,10 +7194,10 @@
       </c>
       <c r="D3" s="24"/>
       <c r="E3" s="25" t="s">
-        <v>151</v>
+        <v>81</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -7541,7 +7215,7 @@
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="T3" s="9" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="U3" s="7"/>
       <c r="V3" s="6" t="s">
@@ -7558,7 +7232,7 @@
       </c>
       <c r="D4" s="24"/>
       <c r="E4" s="25" t="s">
-        <v>152</v>
+        <v>82</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>38</v>
@@ -7572,14 +7246,14 @@
       </c>
       <c r="L4" s="7"/>
       <c r="N4" s="9" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="O4" s="14"/>
       <c r="P4" s="14"/>
       <c r="Q4" s="7"/>
       <c r="R4" s="7"/>
       <c r="T4" s="9" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="U4" s="7"/>
       <c r="V4" s="6" t="s">
@@ -7596,7 +7270,7 @@
       </c>
       <c r="D5" s="24"/>
       <c r="E5" s="25" t="s">
-        <v>153</v>
+        <v>83</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="7"/>
@@ -7608,7 +7282,7 @@
       </c>
       <c r="L5" s="7"/>
       <c r="N5" s="9" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="O5" s="14"/>
       <c r="P5" s="14"/>
@@ -7625,7 +7299,7 @@
       <c r="C6" s="9"/>
       <c r="D6" s="24"/>
       <c r="E6" s="25" t="s">
-        <v>154</v>
+        <v>84</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="7"/>
@@ -7637,7 +7311,7 @@
       </c>
       <c r="L6" s="7"/>
       <c r="N6" s="9" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="O6" s="14"/>
       <c r="P6" s="14"/>
@@ -7652,7 +7326,7 @@
       <c r="C7" s="9"/>
       <c r="D7" s="24"/>
       <c r="E7" s="25" t="s">
-        <v>156</v>
+        <v>86</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="7"/>
@@ -7677,7 +7351,7 @@
       <c r="C8" s="9"/>
       <c r="D8" s="24"/>
       <c r="E8" s="25" t="s">
-        <v>157</v>
+        <v>87</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="7"/>
@@ -7702,7 +7376,7 @@
       <c r="C9" s="9"/>
       <c r="D9" s="24"/>
       <c r="E9" s="25" t="s">
-        <v>158</v>
+        <v>88</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="7"/>
@@ -7894,7 +7568,7 @@
       <c r="I17" s="7"/>
       <c r="J17" s="4"/>
       <c r="K17" s="9" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="L17" s="7"/>
       <c r="N17" s="9"/>

</xml_diff>